<commit_message>
# Load : insert persian number in rhandontable
* not fully completed
</commit_message>
<xml_diff>
--- a/Data_P2.xlsx
+++ b/Data_P2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ardalanmirshani/Dropbox/OCC/Shiny Templates/Shiny apps/Templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ardalanmirshani/Dropbox/RAAVI/RAAVI-Released/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -137,6 +137,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-3000401]0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -166,8 +169,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,7 +468,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -508,11 +512,11 @@
       <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2">
-        <v>15.6</v>
-      </c>
-      <c r="C2">
-        <v>19.600000000000001</v>
+      <c r="B2" s="1">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1">
+        <v>15</v>
       </c>
       <c r="D2">
         <v>17</v>
@@ -543,8 +547,8 @@
       <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3">
-        <v>18</v>
+      <c r="B3" s="1">
+        <v>13</v>
       </c>
       <c r="C3">
         <v>16.5</v>

</xml_diff>